<commit_message>
Initial 50 MeV Ta activation experiment commit. Data through the calibration.
</commit_message>
<xml_diff>
--- a/Experiments/Activation/50MeVTa/CalibrationSources.xlsx
+++ b/Experiments/Activation/50MeVTa/CalibrationSources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -15,23 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Source</t>
-  </si>
-  <si>
-    <r>
-      <t>Initial Activity [</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>μ]</t>
-    </r>
   </si>
   <si>
     <r>
@@ -85,6 +71,23 @@
   </si>
   <si>
     <t xml:space="preserve">Co60     </t>
+  </si>
+  <si>
+    <r>
+      <t>Initial Activity [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μCi]</t>
+    </r>
+  </si>
+  <si>
+    <t>Relative Uncertainty</t>
   </si>
 </sst>
 </file>
@@ -433,107 +436,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>10.3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <f>0.03/2.575</f>
+        <v>1.1650485436893203E-2</v>
+      </c>
+      <c r="D2" s="1">
         <v>25569</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <f>432.6*31540000</f>
         <v>13644204000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1.0620000000000001</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <f t="shared" ref="C3:C7" si="0">0.03/2.575</f>
+        <v>1.1650485436893203E-2</v>
+      </c>
+      <c r="D3" s="1">
         <v>39814</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>13.517*31540000</f>
         <v>426326180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1.0069999999999999</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.1650485436893203E-2</v>
+      </c>
+      <c r="D4" s="1">
         <v>39814</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>1925.28*24*3600</f>
         <v>166344192</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1.042</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.1650485436893203E-2</v>
+      </c>
+      <c r="D5" s="1">
         <v>39814</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>30.08*31540000</f>
         <v>948723200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1.0780000000000001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.1650485436893203E-2</v>
+      </c>
+      <c r="D6" s="1">
         <v>39814</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>10.551*31540000</f>
         <v>332778540</v>
       </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -543,28 +573,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>661.65700000000004</v>
@@ -575,7 +605,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1173.23</v>
@@ -586,7 +616,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1332.49</v>
@@ -600,10 +630,10 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>121.7</v>
+        <v>80.997900000000001</v>
       </c>
       <c r="C5">
-        <v>0.2853</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -611,10 +641,10 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>244.7</v>
+        <v>276.39999999999998</v>
       </c>
       <c r="C6">
-        <v>7.5499999999999998E-2</v>
+        <v>7.1599999999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -622,10 +652,10 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>344.29</v>
+        <v>302.85000000000002</v>
       </c>
       <c r="C7">
-        <v>0.26590000000000003</v>
+        <v>0.18340000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -633,76 +663,87 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>778.9</v>
+        <v>356.01</v>
       </c>
       <c r="C8">
-        <v>0.1293</v>
+        <v>0.62049999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>964.06</v>
+        <v>121.7</v>
       </c>
       <c r="C9">
-        <v>0.14510000000000001</v>
+        <v>0.2853</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1112.08</v>
+        <v>244.7</v>
       </c>
       <c r="C10">
-        <v>0.13669999999999999</v>
+        <v>7.5499999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>1408.01</v>
+        <v>344.29</v>
       </c>
       <c r="C11">
-        <v>0.2087</v>
+        <v>0.26590000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>80.997900000000001</v>
+        <v>778.9</v>
       </c>
       <c r="C12">
-        <v>0.32900000000000001</v>
+        <v>0.1293</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>276.39999999999998</v>
+        <v>964.06</v>
       </c>
       <c r="C13">
-        <v>7.1599999999999997E-2</v>
+        <v>0.14510000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>356.01</v>
+        <v>1112.08</v>
       </c>
       <c r="C14">
-        <v>0.62049999999999994</v>
+        <v>0.13669999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>1408.01</v>
+      </c>
+      <c r="C15">
+        <v>0.2087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>